<commit_message>
complete course detail client
</commit_message>
<xml_diff>
--- a/f4education/backend/Book1.xlsx
+++ b/f4education/backend/Book1.xlsx
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Làm thế nào……</t>
-  </si>
-  <si>
-    <t>Answer One</t>
-  </si>
-  <si>
-    <t>Answer Two</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Answer Three</t>
   </si>
@@ -48,6 +39,72 @@
   </si>
   <si>
     <t>đúng/sai</t>
+  </si>
+  <si>
+    <t>Dùng eclipse</t>
+  </si>
+  <si>
+    <t>Dùng VSCode</t>
+  </si>
+  <si>
+    <t>Dùng Intellij</t>
+  </si>
+  <si>
+    <t>Dùng website chính thứ của spring boot</t>
+  </si>
+  <si>
+    <t>Chạy bằng STS</t>
+  </si>
+  <si>
+    <t>Chạy bằng pring boot dashboard</t>
+  </si>
+  <si>
+    <t>Không biết</t>
+  </si>
+  <si>
+    <t>Không biết nốt</t>
+  </si>
+  <si>
+    <t>foreach + CTRL + spacebar</t>
+  </si>
+  <si>
+    <t>foreach +  spacebar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm sao để tạo project Spring boot </t>
+  </si>
+  <si>
+    <t>Làm sao để chạy project Spring boot</t>
+  </si>
+  <si>
+    <t>Làm sao để chạy foreach project Spring boot</t>
+  </si>
+  <si>
+    <t>Làm sao để tạo một endpoint project Spring boot</t>
+  </si>
+  <si>
+    <t>Tạo trong controller</t>
+  </si>
+  <si>
+    <t>Tạo service controller</t>
+  </si>
+  <si>
+    <t>Tạo trong Model controller</t>
+  </si>
+  <si>
+    <t>Tạo trong repository controller</t>
+  </si>
+  <si>
+    <t>IDE dùng để lập trình Spring boot</t>
+  </si>
+  <si>
+    <t>VSCODE</t>
+  </si>
+  <si>
+    <t>ECLIPSE</t>
+  </si>
+  <si>
+    <t>Intelij</t>
   </si>
 </sst>
 </file>
@@ -86,7 +143,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -368,72 +425,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>